<commit_message>
Handing TimeCellValue with E notation (#359)
</commit_message>
<xml_diff>
--- a/test/test_resources/dataTypesUsingMsExcel365Desktop.xlsx
+++ b/test/test_resources/dataTypesUsingMsExcel365Desktop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catherine\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\excel\test\test_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA0FA5F3-496F-47B0-A1EC-0F7D3492B20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C20E89-23AD-4519-B687-92F21E72F5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{0E801C67-6CD3-4976-BDFB-8C130D7EB2EC}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{0E801C67-6CD3-4976-BDFB-8C130D7EB2EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Text</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>This document has been created using the Microsoft Excel 365 App on Windows at 2023-11 (German, EUR)</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -115,16 +118,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -140,9 +144,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -180,7 +184,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -286,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -428,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -436,23 +440,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FEECBC-B902-4179-8E39-A6DDFF774F6F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -460,7 +464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -468,7 +472,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -476,7 +480,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -484,7 +488,7 @@
         <v>45036</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -492,7 +496,7 @@
         <v>45036.655706018515</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -500,7 +504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -508,7 +512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -516,12 +520,20 @@
         <v>15.99</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>9.7337962962962959E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>